<commit_message>
cvs and other details added
</commit_message>
<xml_diff>
--- a/DAY 3/Leads Accumulation.xlsx
+++ b/DAY 3/Leads Accumulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MARKETING\Documents\GitHub\company-and-personal\DAY 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92219816-3B8B-49C0-B8A7-983E6F32B622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAED3CF5-8454-4013-AE77-D784293FDA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2090" uniqueCount="1050">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2158" uniqueCount="1118">
   <si>
     <t>No</t>
   </si>
@@ -3401,6 +3401,212 @@
   </si>
   <si>
     <t>companyregistration247.com</t>
+  </si>
+  <si>
+    <t>+263 78 991 6802</t>
+  </si>
+  <si>
+    <t>info@sokho-entertainment.com</t>
+  </si>
+  <si>
+    <t>sokho-entertainment.com</t>
+  </si>
+  <si>
+    <t>SOKHO is a full-service entertainment &amp; DJ company based in Harare specializing mostly in WEDDINGS b</t>
+  </si>
+  <si>
+    <t>+263 77 293 4277</t>
+  </si>
+  <si>
+    <t>4 Th Floor LAPF Center, Corner Jason Moyo &amp; Chinhoyi Street, Harare, Zimbabwe</t>
+  </si>
+  <si>
+    <t>info@icdit.org</t>
+  </si>
+  <si>
+    <t>icdit.org</t>
+  </si>
+  <si>
+    <t>Harare Based ICT Training Institution, 100% Hands On Experience in our Fully Equipped Computer Lab</t>
+  </si>
+  <si>
+    <t>+263 78 322 9595</t>
+  </si>
+  <si>
+    <t>admin@inclusive.co.zw</t>
+  </si>
+  <si>
+    <t>62 Bank Street corner Cameroon , Shawasha Hills, Zimbabwe</t>
+  </si>
+  <si>
+    <t>We are your partner in research and management training</t>
+  </si>
+  <si>
+    <t>+263 24 2884709</t>
+  </si>
+  <si>
+    <t>No 56 Edinburgh Road Borrowdale, Harare, Zimbabwe</t>
+  </si>
+  <si>
+    <t>tendernoticeboard@gmail.com</t>
+  </si>
+  <si>
+    <t>tendernoticeboard.co.zw</t>
+  </si>
+  <si>
+    <t>Tender Noticeboard is the trending digital Platform for Tenders and Procurement</t>
+  </si>
+  <si>
+    <t>+263 77 788 3171</t>
+  </si>
+  <si>
+    <t>tondechinde@gmail.com</t>
+  </si>
+  <si>
+    <t>Shop Number 4 Centric Mall Rezende Street (Mt Pleasant Rank), Harare, Zimbabwe</t>
+  </si>
+  <si>
+    <t>Baby essentials and diapers.---- Delivery in Harare for orders above $20 --- Pick up point- Shop 4 C</t>
+  </si>
+  <si>
+    <t>+263 24 2884743</t>
+  </si>
+  <si>
+    <t>12 Cosham road, Borrowdale, Harare, Zimbabwe</t>
+  </si>
+  <si>
+    <t>admin@ptc.ac.zw</t>
+  </si>
+  <si>
+    <t>ptc.ac.zw/contact-us</t>
+  </si>
+  <si>
+    <t>The Leading home school centre in Zimbabwe</t>
+  </si>
+  <si>
+    <t>+263 77 326 9813</t>
+  </si>
+  <si>
+    <t>91 Livingstone ave, Harare, Zimbabwe</t>
+  </si>
+  <si>
+    <t>We have excellent quality rugs, cushions, center tables, dining Suites, headboards and home Decor</t>
+  </si>
+  <si>
+    <t>+263 78 133 1731</t>
+  </si>
+  <si>
+    <t>helpdesk@innbucks.co.zw</t>
+  </si>
+  <si>
+    <t>innbucks.co.zw</t>
+  </si>
+  <si>
+    <t>The Future of Money</t>
+  </si>
+  <si>
+    <t>+263 71 912 7489</t>
+  </si>
+  <si>
+    <t>designs@plusdefoi.co.zw</t>
+  </si>
+  <si>
+    <t>Shop No. B03 Shoppers City Mall, Corner First &amp; Nelson Mandela Street, Harare, Zimbabwe</t>
+  </si>
+  <si>
+    <t>We offer a wide range of branding services from Digital printing, large format printing, engraving, 3D printing, outdoor printing, corporate gifts among others</t>
+  </si>
+  <si>
+    <t>+263 77 824 2258</t>
+  </si>
+  <si>
+    <t>visionshumba33@gmail.com</t>
+  </si>
+  <si>
+    <t>securetracksolutions.co.zw</t>
+  </si>
+  <si>
+    <t>Shop No.7 Kopje Plaza, corner Jason Moyo and Kaguvi, Harare Zimbabwe, Harare, Zimbabwe</t>
+  </si>
+  <si>
+    <t>Assets GPS tracking company from Large vehicles to as small as a Laptop.</t>
+  </si>
+  <si>
+    <t>+263 71 733 5275</t>
+  </si>
+  <si>
+    <t>cityschool03@gmail.com</t>
+  </si>
+  <si>
+    <t>130 Harare St, Thompson House, Corner Speke Avenue and Harare Street, Harare</t>
+  </si>
+  <si>
+    <t>Offering HEXCO courses in Electrical Power Engineering /// Trade Testing Electrical Trade /// Test Preparation (class 1 - 2)</t>
+  </si>
+  <si>
+    <t>hacro@africansunhotels.com</t>
+  </si>
+  <si>
+    <t>africansunhotels.com</t>
+  </si>
+  <si>
+    <t>Bally House, Mount Pleasant Business Park, Cnr. Norfolk Road/870 Endeavor Crescent, Harare, Zimbabwe</t>
+  </si>
+  <si>
+    <t>Welcome to the leading hotel asset management company in Zimbabwe. Whether its business or leisure you're after in Africa, we've got you covered.</t>
+  </si>
+  <si>
+    <t>+263 71 945 6442</t>
+  </si>
+  <si>
+    <t>vestasgarden.co.zw</t>
+  </si>
+  <si>
+    <t>54 Potter Road Waterfalls</t>
+  </si>
+  <si>
+    <t>Vesta's Garden located in Harare, Waterfalls on a private
+homestead, with well maintained
+gardens</t>
+  </si>
+  <si>
+    <t>+263 77 715 0441</t>
+  </si>
+  <si>
+    <t>info@vvg.co.zw</t>
+  </si>
+  <si>
+    <t>vvg.co.zw</t>
+  </si>
+  <si>
+    <t>Shop No.15, First Floor, White House, Corner Cameroon &amp; Albion, Harare, Zimbabwe</t>
+  </si>
+  <si>
+    <t>We specialise in Graphic Design, Website Design, Online Marketing, Advertising, Printing and Compreh</t>
+  </si>
+  <si>
+    <t>+263 77 341 6104</t>
+  </si>
+  <si>
+    <t>robertchihota@gmail.com</t>
+  </si>
+  <si>
+    <t>We provide consultancy services &amp; solutions to Microfinance Institutions (MFIs), and SMEs. We also hope to provide a platform for industry players to share and exchange information, and also discuss Topical Industry Issues</t>
+  </si>
+  <si>
+    <t>+263 24 2257030</t>
+  </si>
+  <si>
+    <t>admin@deutscheschule.co.zw</t>
+  </si>
+  <si>
+    <t>deutscheschule.co.zw</t>
+  </si>
+  <si>
+    <t>No. 9 Lincoln Road Avondale Harare, Harare, Zimbabwe</t>
+  </si>
+  <si>
+    <t>The most reputable German language school in Zimbabwe. Our students sit for Goethe Institute Exams.</t>
   </si>
 </sst>
 </file>
@@ -3765,7 +3971,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -4051,6 +4257,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4388,8 +4609,8 @@
   <dimension ref="A1:Q740"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C153" sqref="C153"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B168" sqref="B168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="12.75"/>
@@ -9545,383 +9766,503 @@
       <c r="P151" s="14"/>
       <c r="Q151" s="14"/>
     </row>
-    <row r="152" spans="1:17" ht="15" customHeight="1">
-      <c r="A152" s="74">
+    <row r="152" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A152" s="11">
         <v>151</v>
       </c>
-      <c r="B152" s="75" t="s">
+      <c r="B152" s="14" t="s">
         <v>524</v>
       </c>
-      <c r="C152" s="75"/>
-      <c r="D152" s="76"/>
-      <c r="E152" s="75"/>
-      <c r="F152" s="74"/>
-      <c r="G152" s="77"/>
-      <c r="H152" s="75"/>
-      <c r="I152" s="75"/>
-      <c r="J152" s="75"/>
-      <c r="K152" s="75"/>
-      <c r="L152" s="75"/>
-      <c r="M152" s="75" t="s">
-        <v>22</v>
-      </c>
-      <c r="N152" s="74" t="s">
-        <v>23</v>
-      </c>
-      <c r="O152" s="75"/>
-      <c r="P152" s="75"/>
-      <c r="Q152" s="75"/>
-    </row>
-    <row r="153" spans="1:17" ht="15" customHeight="1">
-      <c r="A153" s="74">
+      <c r="C152" s="34" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D152" s="90" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E152" s="90" t="s">
+        <v>1050</v>
+      </c>
+      <c r="F152" s="11"/>
+      <c r="G152" s="90" t="s">
+        <v>1053</v>
+      </c>
+      <c r="H152" s="14"/>
+      <c r="I152" s="14"/>
+      <c r="J152" s="14"/>
+      <c r="K152" s="14"/>
+      <c r="L152" s="14"/>
+      <c r="M152" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N152" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O152" s="14"/>
+      <c r="P152" s="14"/>
+      <c r="Q152" s="14"/>
+    </row>
+    <row r="153" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A153" s="11">
         <v>152</v>
       </c>
-      <c r="B153" s="75" t="s">
+      <c r="B153" s="14" t="s">
         <v>525</v>
       </c>
-      <c r="C153" s="75"/>
-      <c r="D153" s="76"/>
-      <c r="E153" s="75"/>
-      <c r="F153" s="74"/>
-      <c r="G153" s="77"/>
-      <c r="H153" s="75"/>
-      <c r="I153" s="75"/>
-      <c r="J153" s="75"/>
-      <c r="K153" s="75"/>
-      <c r="L153" s="75"/>
-      <c r="M153" s="75" t="s">
-        <v>22</v>
-      </c>
-      <c r="N153" s="74" t="s">
-        <v>23</v>
-      </c>
-      <c r="O153" s="75"/>
-      <c r="P153" s="75"/>
-      <c r="Q153" s="75"/>
-    </row>
-    <row r="154" spans="1:17" ht="15" customHeight="1">
-      <c r="A154" s="74">
+      <c r="C153" s="34" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D153" s="90" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E153" s="90" t="s">
+        <v>1054</v>
+      </c>
+      <c r="F153" s="90" t="s">
+        <v>1055</v>
+      </c>
+      <c r="G153" s="90" t="s">
+        <v>1058</v>
+      </c>
+      <c r="H153" s="14"/>
+      <c r="I153" s="14"/>
+      <c r="J153" s="14"/>
+      <c r="K153" s="14"/>
+      <c r="L153" s="14"/>
+      <c r="M153" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N153" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O153" s="14"/>
+      <c r="P153" s="14"/>
+      <c r="Q153" s="14"/>
+    </row>
+    <row r="154" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A154" s="11">
         <v>153</v>
       </c>
-      <c r="B154" s="75" t="s">
+      <c r="B154" s="14" t="s">
         <v>526</v>
       </c>
-      <c r="C154" s="75"/>
-      <c r="D154" s="76"/>
-      <c r="E154" s="75"/>
-      <c r="F154" s="74"/>
-      <c r="G154" s="77"/>
-      <c r="H154" s="75"/>
-      <c r="I154" s="75"/>
-      <c r="J154" s="75"/>
-      <c r="K154" s="75"/>
-      <c r="L154" s="75"/>
-      <c r="M154" s="75" t="s">
-        <v>22</v>
-      </c>
-      <c r="N154" s="74" t="s">
-        <v>23</v>
-      </c>
-      <c r="O154" s="75"/>
-      <c r="P154" s="75"/>
-      <c r="Q154" s="75"/>
-    </row>
-    <row r="155" spans="1:17" ht="15" customHeight="1">
-      <c r="A155" s="74">
+      <c r="C154" s="14"/>
+      <c r="D154" s="90" t="s">
+        <v>1060</v>
+      </c>
+      <c r="E154" s="90" t="s">
+        <v>1059</v>
+      </c>
+      <c r="F154" s="90" t="s">
+        <v>1061</v>
+      </c>
+      <c r="G154" s="90" t="s">
+        <v>1062</v>
+      </c>
+      <c r="H154" s="14"/>
+      <c r="I154" s="14"/>
+      <c r="J154" s="14"/>
+      <c r="K154" s="14"/>
+      <c r="L154" s="14"/>
+      <c r="M154" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N154" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O154" s="14"/>
+      <c r="P154" s="14"/>
+      <c r="Q154" s="14"/>
+    </row>
+    <row r="155" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A155" s="11">
         <v>154</v>
       </c>
-      <c r="B155" s="75" t="s">
+      <c r="B155" s="14" t="s">
         <v>527</v>
       </c>
-      <c r="C155" s="75"/>
-      <c r="D155" s="76"/>
-      <c r="E155" s="75"/>
-      <c r="F155" s="74"/>
-      <c r="G155" s="77"/>
-      <c r="H155" s="75"/>
-      <c r="I155" s="75"/>
-      <c r="J155" s="75"/>
-      <c r="K155" s="75"/>
-      <c r="L155" s="75"/>
-      <c r="M155" s="75" t="s">
-        <v>22</v>
-      </c>
-      <c r="N155" s="74" t="s">
-        <v>23</v>
-      </c>
-      <c r="O155" s="75"/>
-      <c r="P155" s="75"/>
-      <c r="Q155" s="75"/>
-    </row>
-    <row r="156" spans="1:17" ht="15" customHeight="1">
-      <c r="A156" s="74">
+      <c r="C155" s="34" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D155" s="90" t="s">
+        <v>1065</v>
+      </c>
+      <c r="E155" s="90" t="s">
+        <v>1063</v>
+      </c>
+      <c r="F155" s="90" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G155" s="90" t="s">
+        <v>1067</v>
+      </c>
+      <c r="H155" s="14"/>
+      <c r="I155" s="14"/>
+      <c r="J155" s="14"/>
+      <c r="K155" s="14"/>
+      <c r="L155" s="14"/>
+      <c r="M155" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N155" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O155" s="14"/>
+      <c r="P155" s="14"/>
+      <c r="Q155" s="14"/>
+    </row>
+    <row r="156" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A156" s="11">
         <v>155</v>
       </c>
-      <c r="B156" s="75" t="s">
+      <c r="B156" s="14" t="s">
         <v>528</v>
       </c>
-      <c r="C156" s="75"/>
-      <c r="D156" s="76"/>
-      <c r="E156" s="75"/>
-      <c r="F156" s="74"/>
-      <c r="G156" s="77"/>
-      <c r="H156" s="75"/>
-      <c r="I156" s="75"/>
-      <c r="J156" s="75"/>
-      <c r="K156" s="75"/>
-      <c r="L156" s="75"/>
-      <c r="M156" s="75" t="s">
-        <v>22</v>
-      </c>
-      <c r="N156" s="74" t="s">
-        <v>23</v>
-      </c>
-      <c r="O156" s="75"/>
-      <c r="P156" s="75"/>
-      <c r="Q156" s="75"/>
-    </row>
-    <row r="157" spans="1:17" ht="15" customHeight="1">
-      <c r="A157" s="74">
+      <c r="C156" s="14"/>
+      <c r="D156" s="90" t="s">
+        <v>1069</v>
+      </c>
+      <c r="E156" s="90" t="s">
+        <v>1068</v>
+      </c>
+      <c r="F156" s="90" t="s">
+        <v>1070</v>
+      </c>
+      <c r="G156" s="97" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H156" s="14"/>
+      <c r="I156" s="14"/>
+      <c r="J156" s="14"/>
+      <c r="K156" s="14"/>
+      <c r="L156" s="14"/>
+      <c r="M156" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N156" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O156" s="14"/>
+      <c r="P156" s="14"/>
+      <c r="Q156" s="14"/>
+    </row>
+    <row r="157" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A157" s="11">
         <v>156</v>
       </c>
-      <c r="B157" s="75" t="s">
+      <c r="B157" s="14" t="s">
         <v>529</v>
       </c>
-      <c r="C157" s="75"/>
-      <c r="D157" s="76"/>
-      <c r="E157" s="75"/>
-      <c r="F157" s="74"/>
-      <c r="G157" s="77"/>
-      <c r="H157" s="75"/>
-      <c r="I157" s="75"/>
-      <c r="J157" s="75"/>
-      <c r="K157" s="75"/>
-      <c r="L157" s="75"/>
-      <c r="M157" s="75" t="s">
-        <v>22</v>
-      </c>
-      <c r="N157" s="74" t="s">
-        <v>23</v>
-      </c>
-      <c r="O157" s="75"/>
-      <c r="P157" s="75"/>
-      <c r="Q157" s="75"/>
-    </row>
-    <row r="158" spans="1:17" ht="15" customHeight="1">
-      <c r="A158" s="74">
+      <c r="C157" s="92" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D157" s="90" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E157" s="90" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F157" s="90" t="s">
+        <v>1073</v>
+      </c>
+      <c r="G157" s="90" t="s">
+        <v>1076</v>
+      </c>
+      <c r="H157" s="14"/>
+      <c r="I157" s="14"/>
+      <c r="J157" s="14"/>
+      <c r="K157" s="14"/>
+      <c r="L157" s="14"/>
+      <c r="M157" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N157" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O157" s="14"/>
+      <c r="P157" s="14"/>
+      <c r="Q157" s="14"/>
+    </row>
+    <row r="158" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A158" s="11">
         <v>157</v>
       </c>
-      <c r="B158" s="75" t="s">
+      <c r="B158" s="14" t="s">
         <v>530</v>
       </c>
-      <c r="C158" s="75"/>
-      <c r="D158" s="76"/>
-      <c r="E158" s="75"/>
-      <c r="F158" s="74"/>
-      <c r="G158" s="77"/>
-      <c r="H158" s="75"/>
-      <c r="I158" s="75"/>
-      <c r="J158" s="75"/>
-      <c r="K158" s="75"/>
-      <c r="L158" s="75"/>
-      <c r="M158" s="75" t="s">
-        <v>22</v>
-      </c>
-      <c r="N158" s="74" t="s">
-        <v>23</v>
-      </c>
-      <c r="O158" s="75"/>
-      <c r="P158" s="75"/>
-      <c r="Q158" s="75"/>
-    </row>
-    <row r="159" spans="1:17" ht="15" customHeight="1">
-      <c r="A159" s="74">
+      <c r="C158" s="14"/>
+      <c r="D158" s="19"/>
+      <c r="E158" s="90" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F158" s="90" t="s">
+        <v>1078</v>
+      </c>
+      <c r="G158" s="90" t="s">
+        <v>1079</v>
+      </c>
+      <c r="H158" s="14"/>
+      <c r="I158" s="14"/>
+      <c r="J158" s="14"/>
+      <c r="K158" s="14"/>
+      <c r="L158" s="14"/>
+      <c r="M158" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N158" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O158" s="14"/>
+      <c r="P158" s="14"/>
+      <c r="Q158" s="14"/>
+    </row>
+    <row r="159" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A159" s="11">
         <v>158</v>
       </c>
-      <c r="B159" s="75" t="s">
+      <c r="B159" s="14" t="s">
         <v>531</v>
       </c>
-      <c r="C159" s="75"/>
-      <c r="D159" s="76"/>
-      <c r="E159" s="75"/>
-      <c r="F159" s="74"/>
-      <c r="G159" s="77"/>
-      <c r="H159" s="75"/>
-      <c r="I159" s="75"/>
-      <c r="J159" s="75"/>
-      <c r="K159" s="75"/>
-      <c r="L159" s="75"/>
-      <c r="M159" s="75" t="s">
-        <v>22</v>
-      </c>
-      <c r="N159" s="74" t="s">
-        <v>23</v>
-      </c>
-      <c r="O159" s="75"/>
-      <c r="P159" s="75"/>
-      <c r="Q159" s="75"/>
-    </row>
-    <row r="160" spans="1:17" ht="15" customHeight="1">
-      <c r="A160" s="74">
+      <c r="C159" s="34" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D159" s="90" t="s">
+        <v>1081</v>
+      </c>
+      <c r="E159" s="90" t="s">
+        <v>1080</v>
+      </c>
+      <c r="F159" s="11"/>
+      <c r="G159" s="90" t="s">
+        <v>1083</v>
+      </c>
+      <c r="H159" s="14"/>
+      <c r="I159" s="14"/>
+      <c r="J159" s="14"/>
+      <c r="K159" s="14"/>
+      <c r="L159" s="14"/>
+      <c r="M159" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N159" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O159" s="14"/>
+      <c r="P159" s="14"/>
+      <c r="Q159" s="14"/>
+    </row>
+    <row r="160" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A160" s="11">
         <v>159</v>
       </c>
-      <c r="B160" s="75" t="s">
+      <c r="B160" s="14" t="s">
         <v>532</v>
       </c>
-      <c r="C160" s="75"/>
-      <c r="D160" s="76"/>
-      <c r="E160" s="75"/>
-      <c r="F160" s="74"/>
-      <c r="G160" s="77"/>
-      <c r="H160" s="75"/>
-      <c r="I160" s="75"/>
-      <c r="J160" s="75"/>
-      <c r="K160" s="75"/>
-      <c r="L160" s="75"/>
-      <c r="M160" s="75" t="s">
-        <v>22</v>
-      </c>
-      <c r="N160" s="74" t="s">
-        <v>23</v>
-      </c>
-      <c r="O160" s="75"/>
-      <c r="P160" s="75"/>
-      <c r="Q160" s="75"/>
-    </row>
-    <row r="161" spans="1:17" ht="15" customHeight="1">
-      <c r="A161" s="74">
+      <c r="C160" s="14"/>
+      <c r="D160" s="90" t="s">
+        <v>1085</v>
+      </c>
+      <c r="E160" s="90" t="s">
+        <v>1084</v>
+      </c>
+      <c r="F160" s="109" t="s">
+        <v>1086</v>
+      </c>
+      <c r="G160" s="90" t="s">
+        <v>1087</v>
+      </c>
+      <c r="H160" s="14"/>
+      <c r="I160" s="14"/>
+      <c r="J160" s="14"/>
+      <c r="K160" s="14"/>
+      <c r="L160" s="14"/>
+      <c r="M160" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N160" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O160" s="14"/>
+      <c r="P160" s="14"/>
+      <c r="Q160" s="14"/>
+    </row>
+    <row r="161" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A161" s="11">
         <v>160</v>
       </c>
-      <c r="B161" s="75" t="s">
+      <c r="B161" s="14" t="s">
         <v>533</v>
       </c>
-      <c r="C161" s="75"/>
-      <c r="D161" s="76"/>
-      <c r="E161" s="75"/>
-      <c r="F161" s="74"/>
-      <c r="G161" s="77"/>
-      <c r="H161" s="75"/>
-      <c r="I161" s="75"/>
-      <c r="J161" s="75"/>
-      <c r="K161" s="75"/>
-      <c r="L161" s="75"/>
-      <c r="M161" s="75" t="s">
-        <v>22</v>
-      </c>
-      <c r="N161" s="74" t="s">
-        <v>23</v>
-      </c>
-      <c r="O161" s="75"/>
-      <c r="P161" s="75"/>
-      <c r="Q161" s="75"/>
-    </row>
-    <row r="162" spans="1:17" ht="15" customHeight="1">
-      <c r="A162" s="74">
+      <c r="C161" s="34" t="s">
+        <v>1090</v>
+      </c>
+      <c r="D161" s="90" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E161" s="90" t="s">
+        <v>1088</v>
+      </c>
+      <c r="F161" s="109" t="s">
+        <v>1091</v>
+      </c>
+      <c r="G161" s="90" t="s">
+        <v>1092</v>
+      </c>
+      <c r="H161" s="14"/>
+      <c r="I161" s="14"/>
+      <c r="J161" s="14"/>
+      <c r="K161" s="14"/>
+      <c r="L161" s="14"/>
+      <c r="M161" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N161" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O161" s="14"/>
+      <c r="P161" s="14"/>
+      <c r="Q161" s="14"/>
+    </row>
+    <row r="162" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A162" s="11">
         <v>161</v>
       </c>
-      <c r="B162" s="75" t="s">
+      <c r="B162" s="14" t="s">
         <v>534</v>
       </c>
-      <c r="C162" s="75"/>
-      <c r="D162" s="76"/>
-      <c r="E162" s="75"/>
-      <c r="F162" s="74"/>
-      <c r="G162" s="77"/>
-      <c r="H162" s="75"/>
-      <c r="I162" s="75"/>
-      <c r="J162" s="75"/>
-      <c r="K162" s="75"/>
-      <c r="L162" s="75"/>
-      <c r="M162" s="75" t="s">
-        <v>22</v>
-      </c>
-      <c r="N162" s="74" t="s">
-        <v>23</v>
-      </c>
-      <c r="O162" s="75"/>
-      <c r="P162" s="75"/>
-      <c r="Q162" s="75"/>
-    </row>
-    <row r="163" spans="1:17" ht="15" customHeight="1">
-      <c r="A163" s="74">
+      <c r="C162" s="14"/>
+      <c r="D162" s="90" t="s">
+        <v>1094</v>
+      </c>
+      <c r="E162" s="90" t="s">
+        <v>1093</v>
+      </c>
+      <c r="F162" s="90" t="s">
+        <v>1095</v>
+      </c>
+      <c r="G162" s="97" t="s">
+        <v>1096</v>
+      </c>
+      <c r="H162" s="14"/>
+      <c r="I162" s="14"/>
+      <c r="J162" s="14"/>
+      <c r="K162" s="14"/>
+      <c r="L162" s="14"/>
+      <c r="M162" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N162" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O162" s="14"/>
+      <c r="P162" s="14"/>
+      <c r="Q162" s="14"/>
+    </row>
+    <row r="163" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A163" s="11">
         <v>162</v>
       </c>
-      <c r="B163" s="75" t="s">
+      <c r="B163" s="14" t="s">
         <v>535</v>
       </c>
-      <c r="C163" s="75"/>
-      <c r="D163" s="76"/>
-      <c r="E163" s="75"/>
-      <c r="F163" s="74"/>
-      <c r="G163" s="77"/>
-      <c r="H163" s="75"/>
-      <c r="I163" s="75"/>
-      <c r="J163" s="75"/>
-      <c r="K163" s="75"/>
-      <c r="L163" s="75"/>
-      <c r="M163" s="75" t="s">
-        <v>22</v>
-      </c>
-      <c r="N163" s="74" t="s">
-        <v>23</v>
-      </c>
-      <c r="O163" s="75"/>
-      <c r="P163" s="75"/>
-      <c r="Q163" s="75"/>
-    </row>
-    <row r="164" spans="1:17" ht="15" customHeight="1">
-      <c r="A164" s="74">
+      <c r="C163" s="34" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D163" s="90" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E163" s="14"/>
+      <c r="F163" s="90" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G163" s="90" t="s">
+        <v>1100</v>
+      </c>
+      <c r="H163" s="14"/>
+      <c r="I163" s="14"/>
+      <c r="J163" s="14"/>
+      <c r="K163" s="14"/>
+      <c r="L163" s="14"/>
+      <c r="M163" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N163" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O163" s="14"/>
+      <c r="P163" s="14"/>
+      <c r="Q163" s="14"/>
+    </row>
+    <row r="164" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A164" s="11">
         <v>163</v>
       </c>
-      <c r="B164" s="75" t="s">
+      <c r="B164" s="14" t="s">
         <v>536</v>
       </c>
-      <c r="C164" s="75"/>
-      <c r="D164" s="76"/>
-      <c r="E164" s="75"/>
-      <c r="F164" s="74"/>
-      <c r="G164" s="77"/>
-      <c r="H164" s="75"/>
-      <c r="I164" s="75"/>
-      <c r="J164" s="75"/>
-      <c r="K164" s="75"/>
-      <c r="L164" s="75"/>
-      <c r="M164" s="75" t="s">
-        <v>22</v>
-      </c>
-      <c r="N164" s="74" t="s">
-        <v>23</v>
-      </c>
-      <c r="O164" s="75"/>
-      <c r="P164" s="75"/>
-      <c r="Q164" s="75"/>
-    </row>
-    <row r="165" spans="1:17" ht="15" customHeight="1">
-      <c r="A165" s="74">
+      <c r="C164" s="34" t="s">
+        <v>1102</v>
+      </c>
+      <c r="D164" s="19"/>
+      <c r="E164" s="90" t="s">
+        <v>1101</v>
+      </c>
+      <c r="F164" s="90" t="s">
+        <v>1103</v>
+      </c>
+      <c r="G164" s="97" t="s">
+        <v>1104</v>
+      </c>
+      <c r="H164" s="14"/>
+      <c r="I164" s="14"/>
+      <c r="J164" s="14"/>
+      <c r="K164" s="14"/>
+      <c r="L164" s="14"/>
+      <c r="M164" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N164" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O164" s="14"/>
+      <c r="P164" s="14"/>
+      <c r="Q164" s="14"/>
+    </row>
+    <row r="165" spans="1:17" s="2" customFormat="1" ht="15" customHeight="1">
+      <c r="A165" s="24">
         <v>164</v>
       </c>
-      <c r="B165" s="75" t="s">
+      <c r="B165" s="25" t="s">
         <v>537</v>
       </c>
-      <c r="C165" s="75"/>
-      <c r="D165" s="76"/>
-      <c r="E165" s="75"/>
-      <c r="F165" s="74"/>
-      <c r="G165" s="77"/>
-      <c r="H165" s="75"/>
-      <c r="I165" s="75"/>
-      <c r="J165" s="75"/>
-      <c r="K165" s="75"/>
-      <c r="L165" s="75"/>
-      <c r="M165" s="75" t="s">
-        <v>22</v>
-      </c>
-      <c r="N165" s="74" t="s">
-        <v>23</v>
-      </c>
-      <c r="O165" s="75"/>
-      <c r="P165" s="75"/>
-      <c r="Q165" s="75"/>
+      <c r="C165" s="110" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D165" s="111" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E165" s="111" t="s">
+        <v>1105</v>
+      </c>
+      <c r="F165" s="111" t="s">
+        <v>1108</v>
+      </c>
+      <c r="G165" s="111" t="s">
+        <v>1109</v>
+      </c>
+      <c r="H165" s="25"/>
+      <c r="I165" s="25"/>
+      <c r="J165" s="25"/>
+      <c r="K165" s="25"/>
+      <c r="L165" s="25"/>
+      <c r="M165" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="N165" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="O165" s="25"/>
+      <c r="P165" s="25"/>
+      <c r="Q165" s="25"/>
     </row>
     <row r="166" spans="1:17" ht="15" customHeight="1">
       <c r="A166" s="74">
@@ -9931,10 +10272,16 @@
         <v>538</v>
       </c>
       <c r="C166" s="75"/>
-      <c r="D166" s="76"/>
-      <c r="E166" s="75"/>
+      <c r="D166" s="107" t="s">
+        <v>1111</v>
+      </c>
+      <c r="E166" s="107" t="s">
+        <v>1110</v>
+      </c>
       <c r="F166" s="74"/>
-      <c r="G166" s="77"/>
+      <c r="G166" s="107" t="s">
+        <v>1112</v>
+      </c>
       <c r="H166" s="75"/>
       <c r="I166" s="75"/>
       <c r="J166" s="75"/>
@@ -9957,11 +10304,21 @@
       <c r="B167" s="75" t="s">
         <v>539</v>
       </c>
-      <c r="C167" s="75"/>
-      <c r="D167" s="76"/>
-      <c r="E167" s="75"/>
-      <c r="F167" s="74"/>
-      <c r="G167" s="77"/>
+      <c r="C167" s="108" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D167" s="107" t="s">
+        <v>1114</v>
+      </c>
+      <c r="E167" s="107" t="s">
+        <v>1113</v>
+      </c>
+      <c r="F167" s="107" t="s">
+        <v>1116</v>
+      </c>
+      <c r="G167" s="107" t="s">
+        <v>1117</v>
+      </c>
       <c r="H167" s="75"/>
       <c r="I167" s="75"/>
       <c r="J167" s="75"/>
@@ -21319,10 +21676,19 @@
     <hyperlink ref="C148" r:id="rId58" display="https://premierbilliards.co.zw/?fbclid=IwAR1g44KypFJUTWhug21JShYthkDjdVNDcNlVshVqT0UCZiYSL1ruh-drbYU" xr:uid="{21538B73-284F-49B7-A0B6-3F98DDBB2882}"/>
     <hyperlink ref="C149" r:id="rId59" display="http://www.shandahub.com/?fbclid=IwAR3fmNhpKY-jsyk_DVJbq8qHjySUtKcQ69WoXcnA_ub-ZVb5n9S8DH21Vck" xr:uid="{F53AB1C6-3992-4E1F-8773-0DCD8BA79EBE}"/>
     <hyperlink ref="C151" r:id="rId60" display="http://www.companyregistration247.com/?fbclid=IwAR1cFhI_2sW2K3p4Vxud-G7q82JpGyPlXSxD5Oikljb-4PJFi3pKUm_tV00" xr:uid="{9F144C06-C19B-4C44-9113-8F2B20C33175}"/>
+    <hyperlink ref="C152" r:id="rId61" display="http://sokho-entertainment.com/?fbclid=IwAR0Cv8g7u3KNieblwxaNlS6qAvvwW4OcnQPCl9NzWrWyfJLv-aIv2Qh9zdU" xr:uid="{C7160A41-E5A5-4BB0-AF30-4793FA18D8F6}"/>
+    <hyperlink ref="C153" r:id="rId62" display="http://www.icdit.org/?fbclid=IwAR39y6cFOtujXHArfnazo1GX4YNKdj_wKZ8YyDw84fNJOYUJ3w9ZHIJ1qJg" xr:uid="{17DB751C-BF96-49F5-94DA-82D023006425}"/>
+    <hyperlink ref="C155" r:id="rId63" display="https://tendernoticeboard.co.zw/?fbclid=IwAR0Jpmzzl3VYmp-jlNvhxYzQvhx7iEML7fQ6TufhvNrD9eZSGzOLcj-KXoY" xr:uid="{3F489BD1-2CAE-4DF9-B260-71B19AFC024E}"/>
+    <hyperlink ref="C159" r:id="rId64" display="http://innbucks.co.zw/?fbclid=IwAR1LjnHPMWaQo9vtMNeb8HXRFGqyYdK7KHs8ZkDDwVYPjMUulFEy1DEdo8A" xr:uid="{231C1C9B-12DF-42A1-9609-B4395FB4CEEA}"/>
+    <hyperlink ref="C161" r:id="rId65" display="http://www.securetracksolutions.co.zw/?fbclid=IwAR0zIJPpkvF_-3k_S20omoSVF1oD5c5J0TeJCLn4xGEBaEH1kVXbOU1T9g4" xr:uid="{BB7FA3F2-26AF-4E86-A345-A42F0C390E41}"/>
+    <hyperlink ref="C163" r:id="rId66" display="http://www.africansunhotels.com/?fbclid=IwAR2PJQQ6REN0nlyZIxKocQamRAsmt9DnZ0XCFTbFNKJQNhhJD3APXDu-TJE" xr:uid="{60B73B58-725A-4B1C-84E9-EC416D903931}"/>
+    <hyperlink ref="C164" r:id="rId67" display="https://vestasgarden.co.zw/?fbclid=IwAR3HXfCec5--SZhcCKkn_ubYgbDD4K-hBGkxd1vEZbr9KOCbX8kwwWd30oE" xr:uid="{9AEB4946-EBB2-466B-87A6-65BF8F6E6155}"/>
+    <hyperlink ref="C165" r:id="rId68" display="https://www.vvg.co.zw/?fbclid=IwAR0zIJPpkvF_-3k_S20omoSVF1oD5c5J0TeJCLn4xGEBaEH1kVXbOU1T9g4" xr:uid="{EE6F17F6-5388-4E57-8FC0-A92364A056DB}"/>
+    <hyperlink ref="C167" r:id="rId69" display="http://www.deutscheschule.co.zw/?fbclid=IwAR0rp0ChUC7I7qnTrbjhsa9jxiYI-DMvYgZrG0DjBz24lJZgqxmrNKR5ztU" xr:uid="{A42D9F76-9924-4B7F-ABDA-0DC234674B78}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId61"/>
-  <drawing r:id="rId62"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId70"/>
+  <drawing r:id="rId71"/>
 </worksheet>
 </file>
 

</xml_diff>